<commit_message>
Completed the rest of the design
</commit_message>
<xml_diff>
--- a/user view.xlsx
+++ b/user view.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/601873ec7fc0f7d3/Documents/MUICT Works/YEAR 4/ITCS495 - Special Topics in Databases and Intelligent Systems/Project 1 - Sizzler OODB Database Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="376" documentId="8_{26C2FD38-A263-4163-B353-F55AF18A89C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{382334B7-176B-4E58-9357-E79D37DC68A0}"/>
+  <xr:revisionPtr revIDLastSave="394" documentId="8_{26C2FD38-A263-4163-B353-F55AF18A89C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3D92A240-01DB-4951-88E6-39692BA7A1B0}"/>
   <bookViews>
-    <workbookView xWindow="-13695" yWindow="6435" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="1" xr2:uid="{9804AC4C-0FB4-41EC-AA8F-B5E568106E3E}"/>
+    <workbookView xWindow="-13695" yWindow="6435" windowWidth="21600" windowHeight="11385" xr2:uid="{9804AC4C-0FB4-41EC-AA8F-B5E568106E3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Major User View" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="42">
   <si>
     <t>Data</t>
   </si>
@@ -1415,8 +1415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB14215A-C19C-4D6A-8F6D-2BE0943C366C}">
   <dimension ref="A1:K56"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H56" sqref="H56"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2093,7 +2093,9 @@
       <c r="C42" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D42" s="14"/>
+      <c r="D42" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="E42" s="14"/>
       <c r="F42" s="14"/>
       <c r="G42" s="14" t="s">
@@ -2110,7 +2112,9 @@
       <c r="C43" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D43" s="7"/>
+      <c r="D43" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7" t="s">
@@ -2196,30 +2200,52 @@
       <c r="C48" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D48" s="14"/>
-      <c r="E48" s="14"/>
-      <c r="F48" s="14"/>
+      <c r="D48" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E48" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F48" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="G48" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H48" s="14"/>
-      <c r="I48" s="14"/>
+      <c r="H48" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="I48" s="14" t="s">
+        <v>12</v>
+      </c>
       <c r="J48" s="15"/>
     </row>
     <row r="49" spans="1:11" ht="17.25">
       <c r="A49" s="35"/>
-      <c r="B49" s="6"/>
+      <c r="B49" s="6" t="s">
+        <v>12</v>
+      </c>
       <c r="C49" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D49" s="7"/>
-      <c r="E49" s="7"/>
-      <c r="F49" s="7"/>
+      <c r="D49" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F49" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="G49" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="H49" s="7"/>
-      <c r="I49" s="7"/>
+      <c r="H49" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I49" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="J49" s="8"/>
     </row>
     <row r="50" spans="1:11" ht="18" thickBot="1">
@@ -2233,14 +2259,18 @@
       <c r="D50" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E50" s="17"/>
+      <c r="E50" s="17" t="s">
+        <v>12</v>
+      </c>
       <c r="F50" s="17" t="s">
         <v>12</v>
       </c>
       <c r="G50" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="H50" s="17"/>
+      <c r="H50" s="17" t="s">
+        <v>12</v>
+      </c>
       <c r="I50" s="17" t="s">
         <v>12</v>
       </c>
@@ -2382,7 +2412,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0E35F72-B3C3-4274-9CF4-755A02A97BAE}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>

</xml_diff>